<commit_message>
Updated TestScenarios, Readme and Design Document
Design Document now includes additional assumptions.
TestScenarios now include a list of other Test Cases that should be implemented in Selenium for Testing.
Readme has been updated.
</commit_message>
<xml_diff>
--- a/testScenarios.xlsx
+++ b/testScenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Documents\Reward Insight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791C7F4D-5673-475C-89D0-E1A85B152931}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F14E24D-88AC-4777-B7E0-1278DB2015ED}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{FDFE9201-4421-47B2-A888-96FA4163A61D}"/>
   </bookViews>
@@ -25,23 +25,259 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="79">
   <si>
     <t>Admin Employees</t>
   </si>
   <si>
-    <t>Admiin Assign Performance Review</t>
-  </si>
-  <si>
-    <t>Employee Submit Feedback</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Implemented?</t>
+  </si>
+  <si>
+    <t>test_searchEmployeeByIDValid</t>
+  </si>
+  <si>
+    <t>test_searchEmployeeByIDInvalid</t>
+  </si>
+  <si>
+    <t>test_searchEmployeeByNameValid</t>
+  </si>
+  <si>
+    <t>test_searchEmployeeByNameInvalid</t>
+  </si>
+  <si>
+    <t>test_createEmployee</t>
+  </si>
+  <si>
+    <t>test_deleteEmployee</t>
+  </si>
+  <si>
+    <t>test_editEmployee</t>
+  </si>
+  <si>
+    <t>Search for an Existing Employee by the ID Number.</t>
+  </si>
+  <si>
+    <t>Employee Record is retrieved and the ID matches what was provided.</t>
+  </si>
+  <si>
+    <t>Search for an Employee by an ID Number not associated to an Employee.</t>
+  </si>
+  <si>
+    <t>Employee page is empty.</t>
+  </si>
+  <si>
+    <t>Search for an Existing Employee by their Name.</t>
+  </si>
+  <si>
+    <t>Employee Record is retrieved and the Name matches what was provided.</t>
+  </si>
+  <si>
+    <t>Search for an Employee Name that does not Exist.</t>
+  </si>
+  <si>
+    <t>Create a New Employee, providing all Valid values.</t>
+  </si>
+  <si>
+    <t>Employee is successfully created.</t>
+  </si>
+  <si>
+    <t>Delete an Existing Employee.</t>
+  </si>
+  <si>
+    <t>Employee Record no longer exists.</t>
+  </si>
+  <si>
+    <t>Edit an Existing Employee.</t>
+  </si>
+  <si>
+    <t>Employee Record gets updated successfully.</t>
+  </si>
+  <si>
+    <t>No Records are retrieved.</t>
+  </si>
+  <si>
+    <t>Click the Search Button with the Search Bar Empty.</t>
+  </si>
+  <si>
+    <t>Enter "%%'#/" as an Employee First Name.</t>
+  </si>
+  <si>
+    <t>Enter 124484 as an Employee Surname.</t>
+  </si>
+  <si>
+    <t>Enter "ABCDEF" as an Employee Number.</t>
+  </si>
+  <si>
+    <t>Enter "ABCDEF" as an Employee phone Number</t>
+  </si>
+  <si>
+    <t>Enter an email address with a @ in the Employee email field.</t>
+  </si>
+  <si>
+    <t>The text field is highlighted red.</t>
+  </si>
+  <si>
+    <t>Admin Assign Performance Review</t>
+  </si>
+  <si>
+    <t>The page successfully loads and has two text fields, a dropdown and a submit button.</t>
+  </si>
+  <si>
+    <t>The Employees name is entered with no issues.</t>
+  </si>
+  <si>
+    <t>Enter a valid Employee ID in the Employee to Complete Review Field.</t>
+  </si>
+  <si>
+    <t>Enter a valid Employee Name in the Employee to Complete Review Field.</t>
+  </si>
+  <si>
+    <t>The Employees name is displayed in the field.</t>
+  </si>
+  <si>
+    <t>Enter a invalid Employee ID in the Employee to Complete Review Field.</t>
+  </si>
+  <si>
+    <t>Enter a valid Employee Name in the Employee for Review Field.</t>
+  </si>
+  <si>
+    <t>Enter a valid Employee ID in the Employee for Review Field.</t>
+  </si>
+  <si>
+    <t>Enter a invalid Employee Name in the Employee for Review Field.</t>
+  </si>
+  <si>
+    <t>TS01_TC01</t>
+  </si>
+  <si>
+    <t>TS01_TC02</t>
+  </si>
+  <si>
+    <t>TS01_TC03</t>
+  </si>
+  <si>
+    <t>TS01_TC04</t>
+  </si>
+  <si>
+    <t>TS01_TC05</t>
+  </si>
+  <si>
+    <t>TS01_TC06</t>
+  </si>
+  <si>
+    <t>TS01_TC07</t>
+  </si>
+  <si>
+    <t>TS01_TC08</t>
+  </si>
+  <si>
+    <t>TS01_TC09</t>
+  </si>
+  <si>
+    <t>TS01_TC10</t>
+  </si>
+  <si>
+    <t>TS01_TC11</t>
+  </si>
+  <si>
+    <t>TS01_TC12</t>
+  </si>
+  <si>
+    <t>TS01_TC13</t>
+  </si>
+  <si>
+    <t>TS01_TC14</t>
+  </si>
+  <si>
+    <t>TS02_TC01</t>
+  </si>
+  <si>
+    <t>TS02_TC02</t>
+  </si>
+  <si>
+    <t>TS02_TC03</t>
+  </si>
+  <si>
+    <t>TS02_TC04</t>
+  </si>
+  <si>
+    <t>TS02_TC05</t>
+  </si>
+  <si>
+    <t>TS02_TC06</t>
+  </si>
+  <si>
+    <t>TS02_TC07</t>
+  </si>
+  <si>
+    <t>TS02_TC08</t>
+  </si>
+  <si>
+    <t>TS02_TC09</t>
+  </si>
+  <si>
+    <t>TS02_TC10</t>
+  </si>
+  <si>
+    <t>TS02_TC11</t>
+  </si>
+  <si>
+    <t>The values relate to value in the Employee for Review Field.</t>
+  </si>
+  <si>
+    <t>The Review Periods dropdown is populated when a Employee for Review is added.</t>
+  </si>
+  <si>
+    <t>The Review Periods dropdown is empty when Employee for Review is left blank.</t>
+  </si>
+  <si>
+    <t>The drop down is empty.</t>
+  </si>
+  <si>
+    <t>Click Submit once all fields are populated on the UI.</t>
+  </si>
+  <si>
+    <t>An email is generated and sent to the person in the Employee to Complete Review Field.</t>
+  </si>
+  <si>
+    <t>Click submit when not all the fields are populated on the UI.</t>
+  </si>
+  <si>
+    <t>The Submit button is disabled.</t>
+  </si>
+  <si>
+    <t>Enter "*[][343" into the Search Bar.</t>
+  </si>
+  <si>
+    <t>Navigate to the Assign Performance Review Page.</t>
+  </si>
+  <si>
+    <t>Functional Area</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -69,8 +305,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,30 +622,411 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A8AF64-D109-4B4F-A7C7-238387C4F2F3}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>